<commit_message>
Bucle hasta que solo quede uno
</commit_message>
<xml_diff>
--- a/coords_provincias.xlsx
+++ b/coords_provincias.xlsx
@@ -1248,7 +1248,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>RMA</t>
+          <t>MIN</t>
         </is>
       </c>
     </row>
@@ -1260,7 +1260,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>RMA</t>
+          <t>REC</t>
         </is>
       </c>
     </row>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>GAM</t>
+          <t>MIN</t>
         </is>
       </c>
     </row>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>POM</t>
         </is>
       </c>
     </row>
@@ -1308,7 +1308,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>REC</t>
         </is>
       </c>
     </row>
@@ -1320,7 +1320,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>RMA</t>
+          <t>MIN</t>
         </is>
       </c>
     </row>
@@ -1332,7 +1332,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>RMA</t>
+          <t>MIN</t>
         </is>
       </c>
     </row>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ALL</t>
+          <t>GAM</t>
         </is>
       </c>
     </row>
@@ -1356,7 +1356,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>PAR</t>
+          <t>POM</t>
         </is>
       </c>
     </row>
@@ -1368,7 +1368,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>PAR</t>
+          <t>POM</t>
         </is>
       </c>
     </row>
@@ -1392,7 +1392,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>RMA</t>
+          <t>GAM</t>
         </is>
       </c>
     </row>
@@ -1404,7 +1404,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>RMA</t>
+          <t>REC</t>
         </is>
       </c>
     </row>
@@ -1416,7 +1416,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>RMA</t>
+          <t>REC</t>
         </is>
       </c>
     </row>
@@ -1440,7 +1440,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>RMA</t>
+          <t>GAM</t>
         </is>
       </c>
     </row>
@@ -1452,7 +1452,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>RMA</t>
+          <t>GAM</t>
         </is>
       </c>
     </row>
@@ -1488,7 +1488,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>REC</t>
+          <t>GAM</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Conquista de varias provincias a la vez y bucle de reseteo automatico
</commit_message>
<xml_diff>
--- a/coords_provincias.xlsx
+++ b/coords_provincias.xlsx
@@ -1220,10 +1220,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B22" sqref="B2:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1248,7 +1248,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Al-Lagam</t>
         </is>
       </c>
     </row>
@@ -1260,7 +1265,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>REC</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Al-Lagam</t>
         </is>
       </c>
     </row>
@@ -1272,7 +1282,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Al-Lagam</t>
         </is>
       </c>
     </row>
@@ -1284,7 +1299,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>GAM</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Recreativo de Juerga</t>
         </is>
       </c>
     </row>
@@ -1296,7 +1316,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>POM</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Recreativo de Juerga</t>
         </is>
       </c>
     </row>
@@ -1308,7 +1333,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>REC</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Recreativo de Juerga</t>
         </is>
       </c>
     </row>
@@ -1320,7 +1350,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Real Matriz</t>
         </is>
       </c>
     </row>
@@ -1332,7 +1367,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Real Matriz</t>
         </is>
       </c>
     </row>
@@ -1344,7 +1384,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>GAM</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Real Matriz</t>
         </is>
       </c>
     </row>
@@ -1356,7 +1401,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>POM</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Real Club de Parados</t>
         </is>
       </c>
     </row>
@@ -1368,7 +1418,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>POM</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Real Club de Parados</t>
         </is>
       </c>
     </row>
@@ -1380,7 +1435,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>PAR</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Real Club de Parados</t>
         </is>
       </c>
     </row>
@@ -1392,7 +1452,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>GAM</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Pombo FC</t>
         </is>
       </c>
     </row>
@@ -1404,7 +1469,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>REC</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Pombo FC</t>
         </is>
       </c>
     </row>
@@ -1416,7 +1486,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>REC</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Pombo FC</t>
         </is>
       </c>
     </row>
@@ -1428,7 +1503,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>REC</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Minabo de Kiev</t>
         </is>
       </c>
     </row>
@@ -1440,7 +1520,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>GAM</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Minabo de Kiev</t>
         </is>
       </c>
     </row>
@@ -1452,7 +1537,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>GAM</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Minabo de Kiev</t>
         </is>
       </c>
     </row>
@@ -1464,7 +1554,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>GAM</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Gambote del Norte</t>
         </is>
       </c>
     </row>
@@ -1476,7 +1571,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>POM</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Gambote del Norte</t>
         </is>
       </c>
     </row>
@@ -1488,7 +1588,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>GAM</t>
+          <t>Minabo de Kiev</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Gambote del Norte</t>
         </is>
       </c>
     </row>

</xml_diff>